<commit_message>
add data from manometr
</commit_message>
<xml_diff>
--- a/asset/график.xlsx
+++ b/asset/график.xlsx
@@ -217,62 +217,26 @@
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="ru-RU"/>
   <c:chart>
+    <c:title>
+      <c:layout/>
+    </c:title>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="5.1566337520387799E-2"/>
-          <c:y val="4.1130318480304892E-2"/>
-          <c:w val="0.80859964110961857"/>
-          <c:h val="0.90765217566195022"/>
+          <c:x val="5.1566337520387813E-2"/>
+          <c:y val="4.1130318480304864E-2"/>
+          <c:w val="0.80859964110961868"/>
+          <c:h val="0.90765217566195"/>
         </c:manualLayout>
       </c:layout>
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:ser>
-          <c:idx val="0"/>
+          <c:idx val="1"/>
           <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Лист1!$A$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>bar</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:val>
-            <c:numRef>
-              <c:f>Лист1!$A$2:$A$6</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
           <c:tx>
             <c:strRef>
               <c:f>Лист1!$B$1</c:f>
@@ -284,14 +248,38 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:cat>
+            <c:numLit>
+              <c:formatCode>General</c:formatCode>
+              <c:ptCount val="6"/>
+              <c:pt idx="0">
+                <c:v>0</c:v>
+              </c:pt>
+              <c:pt idx="1">
+                <c:v>1</c:v>
+              </c:pt>
+              <c:pt idx="2">
+                <c:v>2</c:v>
+              </c:pt>
+              <c:pt idx="3">
+                <c:v>3</c:v>
+              </c:pt>
+              <c:pt idx="4">
+                <c:v>4</c:v>
+              </c:pt>
+              <c:pt idx="5">
+                <c:v>5</c:v>
+              </c:pt>
+            </c:numLit>
+          </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Лист1!$B$2:$B$6</c:f>
+              <c:f>Лист1!$B$2:$B$7</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>116</c:v>
+                  <c:v>106</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>220</c:v>
@@ -305,29 +293,33 @@
                 <c:pt idx="4">
                   <c:v>726</c:v>
                 </c:pt>
+                <c:pt idx="5">
+                  <c:v>880</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="203557120"/>
-        <c:axId val="204939264"/>
+        <c:axId val="126300544"/>
+        <c:axId val="126303232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="203557120"/>
+        <c:axId val="126300544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="204939264"/>
+        <c:crossAx val="126303232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="204939264"/>
+        <c:axId val="126303232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -335,7 +327,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="203557120"/>
+        <c:crossAx val="126300544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -348,7 +340,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -677,7 +669,7 @@
   <dimension ref="A1:R7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -704,7 +696,7 @@
         <v>0</v>
       </c>
       <c r="B2">
-        <v>116</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="18.75">

</xml_diff>